<commit_message>
Updated raking and models
</commit_message>
<xml_diff>
--- a/data/race_ethnicity_calculations.xlsx
+++ b/data/race_ethnicity_calculations.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14388\Documents\Fields_COVID-19\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBDA9662-7154-455B-8444-A7C3CC2CFE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1B16AF-5CE8-4D81-871D-B08028C22FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6159637A-CAA0-4CFD-901D-CE5D4DF9A63F}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{6159637A-CAA0-4CFD-901D-CE5D4DF9A63F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Race-ethnicity" sheetId="1" r:id="rId1"/>
+    <sheet name="income" sheetId="2" r:id="rId2"/>
+    <sheet name="location" sheetId="3" r:id="rId3"/>
+    <sheet name="age-groups" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
   <si>
     <t>minority</t>
   </si>
@@ -47,9 +50,6 @@
     <t>percentage of visible minority</t>
   </si>
   <si>
-    <t>percentage of population</t>
-  </si>
-  <si>
     <t>chinese</t>
   </si>
   <si>
@@ -98,9 +98,6 @@
     <t>arab</t>
   </si>
   <si>
-    <t>From survey</t>
-  </si>
-  <si>
     <t>black</t>
   </si>
   <si>
@@ -123,6 +120,87 @@
   </si>
   <si>
     <t>white caucasian</t>
+  </si>
+  <si>
+    <t>total population in Ontario</t>
+  </si>
+  <si>
+    <t>percentage of Province population</t>
+  </si>
+  <si>
+    <t>Population numbers</t>
+  </si>
+  <si>
+    <t>Values to use for survey correction</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>population total</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>15-24</t>
+  </si>
+  <si>
+    <t>25-34</t>
+  </si>
+  <si>
+    <t>35-44</t>
+  </si>
+  <si>
+    <t>45-54</t>
+  </si>
+  <si>
+    <t>55-64</t>
+  </si>
+  <si>
+    <t>Group age</t>
+  </si>
+  <si>
+    <t>Percentage of population</t>
+  </si>
+  <si>
+    <t>65 and over</t>
+  </si>
+  <si>
+    <t>Pop. Totals</t>
+  </si>
+  <si>
+    <t>Household income range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt; 15,000 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,000 - 24,999 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">25,000 - 39,999 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">40,000- 59,999 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">60,000 - 89,999 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;90,000 </t>
+  </si>
+  <si>
+    <t>Private households in Ontario</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>All other cities</t>
   </si>
 </sst>
 </file>
@@ -177,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -187,6 +265,9 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,16 +585,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB06EFC-3862-411E-BC32-883AA2DD2F22}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.33203125" customWidth="1"/>
-    <col min="2" max="2" width="34.77734375" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
     <col min="6" max="6" width="27.5546875" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -524,10 +607,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -541,8 +627,12 @@
         <f>B2*G2</f>
         <v>8.6727999999999986E-2</v>
       </c>
+      <c r="D2" s="8">
+        <f>C2*$G$7</f>
+        <v>1166360.9876319999</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2">
         <v>0.29299999999999998</v>
@@ -550,7 +640,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="6">
         <v>0.19400000000000001</v>
@@ -559,8 +649,12 @@
         <f>B3*G2</f>
         <v>5.6841999999999997E-2</v>
       </c>
+      <c r="D3" s="8">
+        <f t="shared" ref="D3:D13" si="0">C3*$G$7</f>
+        <v>764439.29594799993</v>
+      </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3">
         <f>1-G2</f>
@@ -569,7 +663,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="6">
         <v>8.0000000000000002E-3</v>
@@ -578,10 +672,14 @@
         <f>B4*G2</f>
         <v>2.3439999999999997E-3</v>
       </c>
+      <c r="D4" s="8">
+        <f t="shared" si="0"/>
+        <v>31523.269935999997</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="6">
         <v>2.3E-2</v>
@@ -590,10 +688,14 @@
         <f>B5*G2</f>
         <v>6.7389999999999993E-3</v>
       </c>
+      <c r="D5" s="8">
+        <f t="shared" si="0"/>
+        <v>90629.401065999991</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="6">
         <v>3.4000000000000002E-2</v>
@@ -602,10 +704,14 @@
         <f>B6*G2</f>
         <v>9.9620000000000004E-3</v>
       </c>
+      <c r="D6" s="8">
+        <f t="shared" si="0"/>
+        <v>133973.89722800002</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="6">
         <v>0.08</v>
@@ -614,10 +720,20 @@
         <f>B7*G2</f>
         <v>2.3439999999999999E-2</v>
       </c>
+      <c r="D7" s="8">
+        <f t="shared" si="0"/>
+        <v>315232.69935999997</v>
+      </c>
+      <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="7">
+        <v>13448494</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="6">
         <v>0.16200000000000001</v>
@@ -626,10 +742,14 @@
         <f>B8*G2</f>
         <v>4.7466000000000001E-2</v>
       </c>
+      <c r="D8" s="8">
+        <f t="shared" si="0"/>
+        <v>638346.21620400005</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="6">
         <v>0.05</v>
@@ -638,10 +758,14 @@
         <f>B9*G2</f>
         <v>1.465E-2</v>
       </c>
+      <c r="D9" s="8">
+        <f t="shared" si="0"/>
+        <v>197020.43710000001</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="6">
         <v>5.3999999999999999E-2</v>
@@ -650,10 +774,14 @@
         <f>B10*G2</f>
         <v>1.5821999999999999E-2</v>
       </c>
+      <c r="D10" s="8">
+        <f t="shared" si="0"/>
+        <v>212782.07206799998</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="6">
         <v>0.04</v>
@@ -662,10 +790,14 @@
         <f>B11*G2</f>
         <v>1.172E-2</v>
       </c>
+      <c r="D11" s="8">
+        <f t="shared" si="0"/>
+        <v>157616.34967999998</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="6">
         <v>2.5000000000000001E-2</v>
@@ -674,10 +806,14 @@
         <f>B12*G2</f>
         <v>7.3249999999999999E-3</v>
       </c>
+      <c r="D12" s="8">
+        <f t="shared" si="0"/>
+        <v>98510.218550000005</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="6">
         <v>3.3000000000000002E-2</v>
@@ -686,10 +822,14 @@
         <f>B13*G2</f>
         <v>9.6690000000000005E-3</v>
       </c>
+      <c r="D13" s="8">
+        <f t="shared" si="0"/>
+        <v>130033.488486</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="4">
         <f>SUM(B2:B13)</f>
@@ -700,104 +840,446 @@
         <v>0.29270699999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="5">
         <f>C10</f>
         <v>1.5821999999999999E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26" s="8">
+        <f>D10</f>
+        <v>212782.07206799998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B27" s="5">
         <f>C8</f>
         <v>4.7466000000000001E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27" s="8">
+        <f>D8</f>
+        <v>638346.21620400005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B28" s="5">
         <f>C3+C4+C5</f>
         <v>6.5924999999999997E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28" s="8">
+        <f>D3+D4+D5</f>
+        <v>886591.96694999991</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B29" s="3">
         <v>2.8000000000000001E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29" s="8">
+        <f>G7*0.028</f>
+        <v>376557.83199999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B30" s="5">
         <f>C9</f>
         <v>1.465E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30" s="8">
+        <f>D9</f>
+        <v>197020.43710000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B31" s="5">
         <f>C13</f>
         <v>9.6690000000000005E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31" s="8">
+        <f>D13</f>
+        <v>130033.488486</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B32" s="5">
         <f>C6+C7+C11+C12</f>
         <v>5.2447000000000001E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32" s="8">
+        <f>D6+D7+D11+D12</f>
+        <v>705333.16481799993</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B33" s="5">
         <f>C2</f>
         <v>8.6727999999999986E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33" s="8">
+        <f>D2</f>
+        <v>1166360.9876319999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B34" s="3">
         <v>0.67800000000000005</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34" s="8">
+        <f>B34*G7</f>
+        <v>9118078.932</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35" s="4">
         <f>SUM(B26:B34)</f>
         <v>0.99870700000000001</v>
+      </c>
+      <c r="C35" s="8">
+        <f>SUM(C26:C34)</f>
+        <v>13431105.097258</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BB4752-36A8-4127-876B-0CD8341C45BC}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="7">
+        <v>5169170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="9">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="C2" s="8">
+        <f>B2*$I$1</f>
+        <v>294642.69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="9">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C3" s="8">
+        <f t="shared" ref="C3:C7" si="0">B3*$I$1</f>
+        <v>387687.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" si="0"/>
+        <v>599623.72000000009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.154</v>
+      </c>
+      <c r="C5" s="8">
+        <f t="shared" si="0"/>
+        <v>796052.17999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="C6" s="8">
+        <f t="shared" si="0"/>
+        <v>1007988.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="C7" s="8">
+        <f t="shared" si="0"/>
+        <v>2083175.5100000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBC79EA1-4111-47D7-ABC0-3033252158BD}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="7">
+        <v>13448494</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="9">
+        <f>1-B3</f>
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="C2" s="8">
+        <f>B2*$H$1</f>
+        <v>10812589.176000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="C3" s="8">
+        <f>B3*$H$1</f>
+        <v>2635904.824</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA47B252-3003-40BB-B9FB-4E5179F2F5EC}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="7">
+        <v>13448494</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="9">
+        <v>0.127</v>
+      </c>
+      <c r="C2" s="8">
+        <f>B2*$G$1</f>
+        <v>1707958.7380000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0.129</v>
+      </c>
+      <c r="C3" s="8">
+        <f t="shared" ref="C3:C7" si="0">B3*$G$1</f>
+        <v>1734855.726</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.128</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" si="0"/>
+        <v>1721407.2320000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="C5" s="8">
+        <f t="shared" si="0"/>
+        <v>2003825.6059999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="C6" s="8">
+        <f t="shared" si="0"/>
+        <v>1842443.6780000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="C7" s="8">
+        <f t="shared" si="0"/>
+        <v>2245898.4980000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="9">
+        <f>SUM(B2:B7)</f>
+        <v>0.83700000000000008</v>
+      </c>
+      <c r="C8" s="8">
+        <f>SUM(C2:C7)</f>
+        <v>11256389.478</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>